<commit_message>
improved unit tests for error values
</commit_message>
<xml_diff>
--- a/ExcelOpsTest-FreeSpireXls/test_data/ExcelOpsErrorValues.xlsx
+++ b/ExcelOpsTest-FreeSpireXls/test_data/ExcelOpsErrorValues.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-OpenSource\CompuMaster.Excel\ExcelOpsTest\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E91EA7A-6D19-48EA-8685-FFA8B0290D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2D0F48-E9DB-4EDE-A14A-B97DCEE24440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -105,10 +108,23 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="SheetNotExists"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -146,9 +162,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -181,26 +197,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,26 +232,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -426,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9725A0-8F61-4143-B2D8-B9609CE24D7F}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
@@ -448,10 +430,14 @@
         <v>#REF!</v>
       </c>
       <c r="D1" t="e">
-        <f>10^1000</f>
+        <f>[1]SheetNotExists!A1</f>
+        <v>#REF!</v>
+      </c>
+      <c r="E1" t="e">
+        <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
-      <c r="E1" t="e">
+      <c r="F1" t="e">
         <f>VALUE("text")</f>
         <v>#VALUE!</v>
       </c>

</xml_diff>